<commit_message>
SPI Arduino - Raspi
</commit_message>
<xml_diff>
--- a/Webseiten-abschreiben.xlsx
+++ b/Webseiten-abschreiben.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Beschreibung</t>
   </si>
@@ -63,15 +63,6 @@
     <t>Benutzt/ Wo</t>
   </si>
   <si>
-    <t>Bildkoordinaten zu Weltkoordinaten</t>
-  </si>
-  <si>
-    <t>https://stackoverflow.com/questions/30502687/image-coordinate-to-world-coordinate-opencv</t>
-  </si>
-  <si>
-    <t>Kann man eigentlich vergessen</t>
-  </si>
-  <si>
     <t>Blumen clustern</t>
   </si>
   <si>
@@ -97,6 +88,9 @@
   </si>
   <si>
     <t>http://robotics.hobbizine.com/raspiduino.html</t>
+  </si>
+  <si>
+    <t>https://github.com/Pi4J/pi4j/blob/master/pi4j-example/src/main/java/SpiExample.java</t>
   </si>
 </sst>
 </file>
@@ -427,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,13 +461,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -505,43 +499,40 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
         <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
         <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B8" r:id="rId2"/>
+    <hyperlink ref="B11" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>